<commit_message>
Updating scripts to run on Maven
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/automationTestData.xlsx
+++ b/src/test/resources/testData/automationTestData.xlsx
@@ -4,15 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="2340" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16860" windowHeight="2340" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="UserDetails" sheetId="1" r:id="rId1"/>
     <sheet name="TestCases" sheetId="2" r:id="rId2"/>
-    <sheet name="TestData" sheetId="3" r:id="rId3"/>
+    <sheet name="Register" sheetId="3" r:id="rId3"/>
+    <sheet name="Login" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="36">
   <si>
     <t>testCaseId</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>regression,smoke,sanity</t>
+  </si>
+  <si>
+    <t>sanity</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -568,10 +574,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="133" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +600,7 @@
     <col min="16" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,14 +640,8 @@
       <c r="M1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -681,15 +681,110 @@
       <c r="M2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>23</v>
+      <c r="H3" s="2">
+        <v>919876543210</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>